<commit_message>
initial doc update based on moh feedback
</commit_message>
<xml_diff>
--- a/SIAL_docs/SIAL_data_dictionary_MAY_2017.xlsx
+++ b/SIAL_docs/SIAL_data_dictionary_MAY_2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="14880" windowHeight="7905"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="14880" windowHeight="7905" firstSheet="19" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="SIAL contents" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,12 @@
   <definedNames>
     <definedName name="_GoBack" localSheetId="3">MOJ_courtcase_events!$B$26</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="522">
   <si>
     <t>Variable name</t>
   </si>
@@ -5786,8 +5786,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5796,8 +5796,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="685800" y="6057900"/>
-          <a:ext cx="9353550" cy="2000250"/>
+          <a:off x="685800" y="6629400"/>
+          <a:ext cx="9353550" cy="4953000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5844,16 +5844,40 @@
             <a:t>Event table description:  </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>We define each chronic condition per person as an individual event. There are no costs associated with these events.</a:t>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Despite the name of this table, which is consistent with the IDI name, this table contains chronic conditions and significant health events . We define each chronic condition/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> significant health event </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>per person as an individual event. There are no costs associated with these events.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5939,6 +5963,222 @@
             </a:rPr>
             <a:t>with other tables. Variable names and types have been standardised .</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-NZ" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> The end date is the last incident date.  For CHD conditions, the fields entitled ‘first incident date’ and ‘most recent incident date’ don’t always represent the first and most recent incident dates. These fields are calculated in a different way to other conditions: </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>*</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The ‘first incident date’ field represents the first date the person received a ‘CHD diagnosis’ (listed above) in NMDS. This may not necessarily be the first incident date as a person may have been dispensed a ‘CHD pharmaceutical’ (listed above) before this date. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>* The ‘most recent date’ field represents the first date the person received a ‘CHD diagnosis’ in NMDS or the first dispensing of a ‘CHD pharmaceutical’. This approach is more comprehensive but uses pharmaceutical data which is less specific and reliable than diagnostic codes. Furthermore the date is unlikely to represent the most recent incident date as the person may have received a “CHD diagnosis/pharmaceutical” after this date. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-NZ" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>According to Dr. Terry Quirke (National Health Committee) the first option is more robust and therefore we recommend that you use the ‘first incident date’ field. However option two is also available if option two is preferred. " </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-NZ" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-NZ">
@@ -6250,8 +6490,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6260,8 +6500,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="723900" y="7991476"/>
-          <a:ext cx="9353550" cy="3676650"/>
+          <a:off x="723900" y="8372476"/>
+          <a:ext cx="9353550" cy="4543424"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6468,7 +6708,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> This data is publically available and is saved in the SIAL dependencies folder.</a:t>
+            <a:t> This data is publically available and is saved in the SIAL dependencies folder. The original cost figures can be found on p70 of http://www.treasury.govt.nz/budget/2014/estimates/v6/est14-v6-health.pdf</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6519,6 +6759,52 @@
             </a:rPr>
             <a:t>be revisited after correct amounts are obtained. </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-NZ" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The Ministry</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> of Health has noted that B4sc costs vary around the country but it is not practical for them to provide cost data below the national level so they are happy with the approached used based on the national average.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -8617,8 +8903,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1828800</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8627,8 +8913,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="657225" y="4619625"/>
-          <a:ext cx="9363075" cy="2343150"/>
+          <a:off x="657225" y="5200650"/>
+          <a:ext cx="9363075" cy="2705100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8838,7 +9124,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>ost 50% of rows are exact duplicates. The quality of this dataset needs to be checked with</a:t>
+            <a:t>ost 50% of rows are exact duplicates. The</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-NZ" sz="1100" baseline="0">
@@ -8850,7 +9136,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> MOH.</a:t>
+            <a:t> Ministry of Health speculated this could be caused by: the IDI joining to dim_vaccine_antigen_dose which would create duplicates or somehow merging partially overlapping extracts. Use of a select distinct removes these duplicates.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -13028,8 +13314,8 @@
   </sheetPr>
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13169,8 +13455,8 @@
       <c r="G6" s="89">
         <v>42736</v>
       </c>
-      <c r="H6" s="89" t="s">
-        <v>420</v>
+      <c r="H6" s="89">
+        <v>42856</v>
       </c>
       <c r="I6" s="89" t="s">
         <v>456</v>
@@ -13559,8 +13845,8 @@
       <c r="G21" s="89">
         <v>42552</v>
       </c>
-      <c r="H21" s="88" t="s">
-        <v>420</v>
+      <c r="H21" s="89">
+        <v>42522</v>
       </c>
       <c r="I21" s="89" t="s">
         <v>455</v>
@@ -13585,8 +13871,8 @@
       <c r="G22" s="89">
         <v>42552</v>
       </c>
-      <c r="H22" s="88" t="s">
-        <v>420</v>
+      <c r="H22" s="89">
+        <v>42522</v>
       </c>
       <c r="I22" s="88" t="s">
         <v>456</v>
@@ -13715,8 +14001,8 @@
       <c r="G27" s="89">
         <v>42552</v>
       </c>
-      <c r="H27" s="88" t="s">
-        <v>420</v>
+      <c r="H27" s="89">
+        <v>42522</v>
       </c>
       <c r="I27" s="89" t="s">
         <v>455</v>
@@ -17027,8 +17313,8 @@
   </sheetPr>
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17265,9 +17551,7 @@
   </sheetPr>
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18499,8 +18783,8 @@
   </sheetPr>
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>